<commit_message>
feat: add inventory system with add/remove item functionality
</commit_message>
<xml_diff>
--- a/Tools/Luban/DataTables/Datas/__enums__.xlsx
+++ b/Tools/Luban/DataTables/Datas/__enums__.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10921"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27932"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangwencheng/UnityProject/2025TTGJ/Tools/Luban/DataTables/Datas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\1_Game_Data\Unity\2025TTGJ\Tools\Luban\DataTables\Datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DFA2D8F-3C53-8444-AD4A-8DAA222EC474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC98398-F1CB-4DA5-8FF3-4F08D663C210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="12960" windowHeight="9380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1640" yWindow="2810" windowWidth="28670" windowHeight="17120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="100">
   <si>
     <t>##var</t>
   </si>
@@ -92,62 +92,306 @@
     <t>注释</t>
   </si>
   <si>
-    <t>test.ETestQuality</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>白</t>
-  </si>
-  <si>
-    <t>最高品质</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>黑</t>
-  </si>
-  <si>
-    <t>黑色的</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>蓝</t>
-  </si>
-  <si>
-    <t>蓝色的</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>红</t>
-  </si>
-  <si>
-    <t>最差品质</t>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>quality</t>
+  </si>
+  <si>
+    <t>品质枚举</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>white</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>green</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>blue</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>purple</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>orange</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>red</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>白品质</t>
+  </si>
+  <si>
+    <t>绿品质</t>
+  </si>
+  <si>
+    <t>蓝品质</t>
+  </si>
+  <si>
+    <t>紫品质</t>
+  </si>
+  <si>
+    <t>橙品质</t>
+  </si>
+  <si>
+    <t>红品质</t>
+  </si>
+  <si>
+    <t>pokemon_Type1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>宝可梦属性</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>一般</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>火</t>
+  </si>
+  <si>
+    <t>Fire</t>
+  </si>
+  <si>
+    <t>水</t>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>草</t>
+  </si>
+  <si>
+    <t>Grass</t>
+  </si>
+  <si>
+    <t>电</t>
+  </si>
+  <si>
+    <t>Electric</t>
+  </si>
+  <si>
+    <t>冰</t>
+  </si>
+  <si>
+    <t>Ice</t>
+  </si>
+  <si>
+    <t>虫</t>
+  </si>
+  <si>
+    <t>Bug</t>
+  </si>
+  <si>
+    <t>飞行</t>
+  </si>
+  <si>
+    <t>Flying</t>
+  </si>
+  <si>
+    <t>地面</t>
+  </si>
+  <si>
+    <t>Ground</t>
+  </si>
+  <si>
+    <t>岩石</t>
+  </si>
+  <si>
+    <t>Rock</t>
+  </si>
+  <si>
+    <t>格斗</t>
+  </si>
+  <si>
+    <t>Fighting</t>
+  </si>
+  <si>
+    <t>超能力</t>
+  </si>
+  <si>
+    <t>Psychic</t>
+  </si>
+  <si>
+    <t>幽灵</t>
+  </si>
+  <si>
+    <t>Ghost</t>
+  </si>
+  <si>
+    <t>毒</t>
+  </si>
+  <si>
+    <t>Poison</t>
+  </si>
+  <si>
+    <t>恶</t>
+  </si>
+  <si>
+    <t>Dark</t>
+  </si>
+  <si>
+    <t>钢</t>
+  </si>
+  <si>
+    <t>Steel</t>
+  </si>
+  <si>
+    <t>龙</t>
+  </si>
+  <si>
+    <t>Dragon</t>
+  </si>
+  <si>
+    <t>妖精</t>
+  </si>
+  <si>
+    <t>Fairy</t>
+  </si>
+  <si>
+    <t>experience_growth</t>
+  </si>
+  <si>
+    <t>宝可梦升级速度</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>​​Erratic​​</t>
+  </si>
+  <si>
+    <t>​​Fast​​</t>
+  </si>
+  <si>
+    <t>​​Medium Fast​​</t>
+  </si>
+  <si>
+    <t>​​Medium Slow​​</t>
+  </si>
+  <si>
+    <t>​​Slow​​</t>
+  </si>
+  <si>
+    <t>​​Fluctuating​​</t>
+  </si>
+  <si>
+    <t>最快,初期升级非常快，但后期所需经验值大幅增加。</t>
+  </si>
+  <si>
+    <t>快,整体升级速度较快，达到100级所需的总经验值相对较少。</t>
+  </si>
+  <si>
+    <t>慢,整体升级速度较慢，需要积累较多的经验值才能升级。</t>
+  </si>
+  <si>
+    <t>最慢,初期升级极慢，但从中期开始升级速度会显著加快</t>
+  </si>
+  <si>
+    <t>较快,升级所需经验值呈平稳的抛物线增长，是最常见的类型之一。</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>较慢,升级曲线较为复杂，前期和中期升级速度适中。</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>map_Type</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>classic</t>
+  </si>
+  <si>
+    <t>Endless</t>
+  </si>
+  <si>
+    <t>经典</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>无尽</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>副本类型</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>map_SubType</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>副本子类型</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>pokemon</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>bossPokemon</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>npc</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>简单宝可梦</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>boss宝可梦</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>npc对战</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -173,19 +417,22 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -458,13 +705,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="8.1640625" customWidth="1"/>
@@ -475,7 +722,7 @@
     <col min="10" max="10" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -497,15 +744,15 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -525,7 +772,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -551,76 +798,571 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="3">
+        <v>1</v>
+      </c>
+      <c r="J5" s="3">
+        <v>1</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="H6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="3">
+        <v>2</v>
+      </c>
+      <c r="J6" s="3">
+        <v>2</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="3">
+        <v>3</v>
+      </c>
+      <c r="J7" s="3">
+        <v>3</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" s="3">
+        <v>4</v>
+      </c>
+      <c r="J8" s="3">
+        <v>4</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L8" s="3"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="3">
+        <v>5</v>
+      </c>
+      <c r="J9" s="3">
+        <v>5</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L9" s="3"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" t="b">
+        <v>1</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" t="s">
+        <v>37</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H11" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11" s="3">
+        <v>1</v>
+      </c>
+      <c r="J11" s="3">
+        <v>1</v>
+      </c>
+      <c r="K11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H12" t="s">
+        <v>41</v>
+      </c>
+      <c r="I12">
+        <v>2</v>
+      </c>
+      <c r="J12">
+        <v>2</v>
+      </c>
+      <c r="K12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H13" t="s">
+        <v>43</v>
+      </c>
+      <c r="I13" s="3">
+        <v>3</v>
+      </c>
+      <c r="J13" s="3">
+        <v>3</v>
+      </c>
+      <c r="K13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H14" t="s">
+        <v>45</v>
+      </c>
+      <c r="I14">
+        <v>4</v>
+      </c>
+      <c r="J14">
+        <v>4</v>
+      </c>
+      <c r="K14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="H5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J5">
+      <c r="H15" t="s">
+        <v>47</v>
+      </c>
+      <c r="I15" s="3">
+        <v>5</v>
+      </c>
+      <c r="J15" s="3">
+        <v>5</v>
+      </c>
+      <c r="K15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H16" t="s">
+        <v>49</v>
+      </c>
+      <c r="I16">
+        <v>6</v>
+      </c>
+      <c r="J16">
+        <v>6</v>
+      </c>
+      <c r="K16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H17" t="s">
+        <v>51</v>
+      </c>
+      <c r="I17" s="3">
+        <v>7</v>
+      </c>
+      <c r="J17" s="3">
+        <v>7</v>
+      </c>
+      <c r="K17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H18" t="s">
+        <v>53</v>
+      </c>
+      <c r="I18">
+        <v>8</v>
+      </c>
+      <c r="J18">
+        <v>8</v>
+      </c>
+      <c r="K18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H19" t="s">
+        <v>55</v>
+      </c>
+      <c r="I19" s="3">
+        <v>9</v>
+      </c>
+      <c r="J19" s="3">
+        <v>9</v>
+      </c>
+      <c r="K19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H20" t="s">
+        <v>57</v>
+      </c>
+      <c r="I20">
+        <v>10</v>
+      </c>
+      <c r="J20">
+        <v>10</v>
+      </c>
+      <c r="K20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H21" t="s">
+        <v>59</v>
+      </c>
+      <c r="I21" s="3">
+        <v>11</v>
+      </c>
+      <c r="J21" s="3">
+        <v>11</v>
+      </c>
+      <c r="K21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H22" t="s">
+        <v>61</v>
+      </c>
+      <c r="I22">
+        <v>12</v>
+      </c>
+      <c r="J22">
+        <v>12</v>
+      </c>
+      <c r="K22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H23" t="s">
+        <v>63</v>
+      </c>
+      <c r="I23" s="3">
+        <v>13</v>
+      </c>
+      <c r="J23" s="3">
+        <v>13</v>
+      </c>
+      <c r="K23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H24" t="s">
+        <v>65</v>
+      </c>
+      <c r="I24">
+        <v>14</v>
+      </c>
+      <c r="J24">
+        <v>14</v>
+      </c>
+      <c r="K24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H25" t="s">
+        <v>67</v>
+      </c>
+      <c r="I25" s="3">
+        <v>15</v>
+      </c>
+      <c r="J25" s="3">
+        <v>15</v>
+      </c>
+      <c r="K25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H26" t="s">
+        <v>69</v>
+      </c>
+      <c r="I26">
+        <v>16</v>
+      </c>
+      <c r="J26">
+        <v>16</v>
+      </c>
+      <c r="K26" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H27" t="s">
+        <v>71</v>
+      </c>
+      <c r="I27" s="3">
+        <v>17</v>
+      </c>
+      <c r="J27" s="3">
+        <v>17</v>
+      </c>
+      <c r="K27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" t="b">
+        <v>0</v>
+      </c>
+      <c r="D28" t="b">
+        <v>1</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H28" t="s">
+        <v>74</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H29" t="s">
+        <v>75</v>
+      </c>
+      <c r="I29" s="3">
+        <v>1</v>
+      </c>
+      <c r="J29" s="3">
+        <v>1</v>
+      </c>
+      <c r="K29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H30" t="s">
+        <v>76</v>
+      </c>
+      <c r="I30">
         <v>2</v>
       </c>
-      <c r="K5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="H6" t="s">
-        <v>26</v>
-      </c>
-      <c r="I6" t="s">
-        <v>27</v>
-      </c>
-      <c r="J6">
+      <c r="J30">
+        <v>2</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H31" t="s">
+        <v>77</v>
+      </c>
+      <c r="I31" s="3">
         <v>3</v>
       </c>
-      <c r="K6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="H7" t="s">
-        <v>29</v>
-      </c>
-      <c r="I7" t="s">
-        <v>30</v>
-      </c>
-      <c r="J7">
+      <c r="J31" s="3">
+        <v>3</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H32" t="s">
+        <v>78</v>
+      </c>
+      <c r="I32">
         <v>4</v>
       </c>
-      <c r="K7" t="s">
-        <v>31</v>
+      <c r="J32">
+        <v>4</v>
+      </c>
+      <c r="K32" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H33" t="s">
+        <v>79</v>
+      </c>
+      <c r="I33" s="3">
+        <v>5</v>
+      </c>
+      <c r="J33" s="3">
+        <v>5</v>
+      </c>
+      <c r="K33" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>86</v>
+      </c>
+      <c r="C34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D34" t="b">
+        <v>1</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H34" t="s">
+        <v>87</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+      <c r="K34" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H35" t="s">
+        <v>88</v>
+      </c>
+      <c r="I35" s="3">
+        <v>1</v>
+      </c>
+      <c r="J35" s="3">
+        <v>1</v>
+      </c>
+      <c r="K35" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>92</v>
+      </c>
+      <c r="C36" t="b">
+        <v>0</v>
+      </c>
+      <c r="D36" t="b">
+        <v>1</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="K36" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H37" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I37" s="3">
+        <v>1</v>
+      </c>
+      <c r="J37" s="3">
+        <v>1</v>
+      </c>
+      <c r="K37" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H38" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="I38">
+        <v>2</v>
+      </c>
+      <c r="J38">
+        <v>2</v>
+      </c>
+      <c r="K38" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="H1:L1"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>

</xml_diff>

<commit_message>
add luban json,card panel
</commit_message>
<xml_diff>
--- a/Tools/Luban/DataTables/Datas/__enums__.xlsx
+++ b/Tools/Luban/DataTables/Datas/__enums__.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangwencheng/UnityProject/2025TTGJ/Tools/Luban/DataTables/Datas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB7A7C2-FF26-0545-B818-38FC95F843D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B730DEB-6AC9-DC40-87AE-32D0E07FA7CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1260" windowWidth="28680" windowHeight="17120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7060" yWindow="2320" windowWidth="28680" windowHeight="17120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -264,24 +264,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>​​Erratic​​</t>
-  </si>
-  <si>
-    <t>​​Fast​​</t>
-  </si>
-  <si>
-    <t>​​Medium Fast​​</t>
-  </si>
-  <si>
-    <t>​​Medium Slow​​</t>
-  </si>
-  <si>
-    <t>​​Slow​​</t>
-  </si>
-  <si>
-    <t>​​Fluctuating​​</t>
-  </si>
-  <si>
     <t>最快,初期升级非常快，但后期所需经验值大幅增加。</t>
   </si>
   <si>
@@ -354,6 +336,24 @@
   <si>
     <t>npc对战</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Erratic</t>
+  </si>
+  <si>
+    <t>Fast</t>
+  </si>
+  <si>
+    <t>Slow</t>
+  </si>
+  <si>
+    <t>Fluctuating</t>
+  </si>
+  <si>
+    <t>MediumFast</t>
+  </si>
+  <si>
+    <t>MediumSlow</t>
   </si>
 </sst>
 </file>
@@ -704,7 +704,7 @@
   <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1163,7 +1163,7 @@
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
+      <c r="B28" s="1" t="s">
         <v>71</v>
       </c>
       <c r="C28" t="b">
@@ -1175,36 +1175,36 @@
       <c r="F28" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H28" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28" t="s">
         <v>73</v>
       </c>
-      <c r="I28">
-        <v>0</v>
-      </c>
-      <c r="J28">
-        <v>0</v>
-      </c>
-      <c r="K28" t="s">
-        <v>79</v>
-      </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="H29" t="s">
+      <c r="H29" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I29" s="2">
+        <v>1</v>
+      </c>
+      <c r="J29" s="2">
+        <v>1</v>
+      </c>
+      <c r="K29" t="s">
         <v>74</v>
       </c>
-      <c r="I29" s="2">
-        <v>1</v>
-      </c>
-      <c r="J29" s="2">
-        <v>1</v>
-      </c>
-      <c r="K29" t="s">
-        <v>80</v>
-      </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="H30" t="s">
-        <v>75</v>
+      <c r="H30" s="1" t="s">
+        <v>97</v>
       </c>
       <c r="I30">
         <v>2</v>
@@ -1213,12 +1213,12 @@
         <v>2</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="H31" t="s">
-        <v>76</v>
+      <c r="H31" s="1" t="s">
+        <v>98</v>
       </c>
       <c r="I31" s="2">
         <v>3</v>
@@ -1227,12 +1227,12 @@
         <v>3</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="H32" t="s">
-        <v>77</v>
+      <c r="H32" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="I32">
         <v>4</v>
@@ -1241,12 +1241,12 @@
         <v>4</v>
       </c>
       <c r="K32" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="H33" t="s">
-        <v>78</v>
+      <c r="H33" s="1" t="s">
+        <v>96</v>
       </c>
       <c r="I33" s="2">
         <v>5</v>
@@ -1255,12 +1255,12 @@
         <v>5</v>
       </c>
       <c r="K33" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C34" t="b">
         <v>0</v>
@@ -1269,10 +1269,10 @@
         <v>1</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="H34" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="I34">
         <v>0</v>
@@ -1281,12 +1281,12 @@
         <v>0</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.2">
       <c r="H35" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="I35" s="2">
         <v>1</v>
@@ -1295,12 +1295,12 @@
         <v>1</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C36" t="b">
         <v>0</v>
@@ -1309,10 +1309,10 @@
         <v>1</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="I36">
         <v>0</v>
@@ -1321,12 +1321,12 @@
         <v>0</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.2">
       <c r="H37" s="2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="I37" s="2">
         <v>1</v>
@@ -1335,12 +1335,12 @@
         <v>1</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.2">
       <c r="H38" s="2" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="I38">
         <v>2</v>
@@ -1349,7 +1349,7 @@
         <v>2</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>